<commit_message>
Updates for SSN risks and their weights and a initial draft for the final weights which can be modified as needed.
</commit_message>
<xml_diff>
--- a/social footprint weight sheet.xlsx
+++ b/social footprint weight sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Attribute</t>
   </si>
@@ -35,10 +35,13 @@
     <t>variable</t>
   </si>
   <si>
-    <t>PII</t>
-  </si>
-  <si>
-    <t>Password recovery</t>
+    <t>cross site</t>
+  </si>
+  <si>
+    <t>ssn risks</t>
+  </si>
+  <si>
+    <t>Total risks (30% to cross site linking/matching + 70% to ssn)</t>
   </si>
   <si>
     <t>Age (Could be synonymous to Birth Year?)</t>
@@ -322,7 +325,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -331,25 +337,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -516,13 +519,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -621,10 +618,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -879,13 +876,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1198,10 +1189,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1461,11 +1452,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="34.3984" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7656" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.0781" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.0781" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.9844" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.3516" style="1" customWidth="1"/>
     <col min="6" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1482,36 +1473,44 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.122</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1519,32 +1518,42 @@
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.155</v>
+      </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.35</v>
+      </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>0.105</v>
+      </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1552,65 +1561,93 @@
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.144</v>
+      </c>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.031</v>
+      </c>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.028</v>
+      </c>
     </row>
     <row r="11" ht="13.65" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.189</v>
+      </c>
     </row>
     <row r="12" ht="13.65" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="13" ht="13.65" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1618,10 +1655,10 @@
     </row>
     <row r="14" ht="13.65" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1629,14 +1666,20 @@
     </row>
     <row r="15" ht="13.65" customHeight="1">
       <c r="A15" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>31</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.056</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1654,22 +1697,20 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="5" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="6" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customHeight="1">
-      <c r="A1" s="6"/>
+      <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>

</xml_diff>